<commit_message>
adicionando collection do postman
</commit_message>
<xml_diff>
--- a/bd/senai_wishlist_desafio_bd_importacao.xlsx
+++ b/bd/senai_wishlist_desafio_bd_importacao.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saulo\Documents\WORKS\SENAI Info\2º Semestre\1s2019\senai_wishlist_desafio\senai_wishlist_desafio\bd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\senai_wishlist_desafio\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TiposUsuarios" sheetId="6" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -623,17 +623,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -641,7 +641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -649,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -670,16 +670,16 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -696,7 +696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -713,7 +713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -730,7 +730,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -747,7 +747,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -764,7 +764,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -781,7 +781,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -798,7 +798,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" s="23"/>
     </row>
   </sheetData>
@@ -819,18 +819,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>9</v>
       </c>
@@ -841,7 +841,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -852,7 +852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -863,7 +863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -874,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -885,7 +885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19">
         <v>5</v>
       </c>

</xml_diff>